<commit_message>
mais perguntas para canis
</commit_message>
<xml_diff>
--- a/dados dos inquéritos.xlsx
+++ b/dados dos inquéritos.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardacunha/Documents/Uni/3/PPIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardacunha/Documents/Uni/3/PPIN/FEUP-PPIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Inquéritos p/ o Projeto de Inovação</t>
   </si>
@@ -125,31 +125,37 @@
     <t>Na sua opinião, o canil em que trabalha/trabalhou está sobrelotado?</t>
   </si>
   <si>
-    <t>No canil em que trabalha/trabalhou , há falta de condições de saneamento para os animais?</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , há falta de alimento para os animais? Têm de racionar?</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , há falta de medicação para os animais? Têm de racionar?</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , como obtêm os alimentos?</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , como obtêm a medicação?</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , os animais recebem cuidados veterinários quando...</t>
-  </si>
-  <si>
-    <t>No canil em que trabalha/trabalhou , os serviços veterinários são pagos por...</t>
-  </si>
-  <si>
     <t>Índice</t>
   </si>
   <si>
     <t>Pergunta</t>
+  </si>
+  <si>
+    <t>Na sua opinião, no canil em que trabalha/trabalhou, há falta de condições de saneamento para os animais?</t>
+  </si>
+  <si>
+    <t>Na sua opinião, no canil em que trabalha/trabalhou, há falta de alimento para os animais? Têm de racionar?</t>
+  </si>
+  <si>
+    <t>Na sua opinião, no canil em que trabalha/trabalhou, há falta de medicação para os animais? Têm de racionar?</t>
+  </si>
+  <si>
+    <t>No canil em que trabalha/trabalhou, como obtêm os alimentos?</t>
+  </si>
+  <si>
+    <t>No canil em que trabalha/trabalhou, como obtêm a medicação?</t>
+  </si>
+  <si>
+    <t>No canil em que trabalha/trabalhou, os animais recebem cuidados veterinários quando...</t>
+  </si>
+  <si>
+    <t>No canil em que trabalha/trabalhou, os serviços veterinários são pagos por...</t>
+  </si>
+  <si>
+    <t>Na sua opinião, no canil em que trabalha/trabalhou, há voluntários/trabalhadores suficientes para o trabalho exigido?</t>
+  </si>
+  <si>
+    <t>Não sei</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +315,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -324,11 +348,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,20 +362,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,9 +397,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,6 +441,30 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6426,797 +6459,839 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="N86" sqref="N86"/>
+      <selection activeCell="R81" sqref="R81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="10.83203125" style="8"/>
-    <col min="4" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="14" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="23.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="14" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="M1" s="4" t="s">
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="M2" s="2">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="2"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="M3" s="2">
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="M3" s="1">
         <v>0</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="O4" s="2"/>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="L5" s="11" t="s">
+      <c r="B5" s="36"/>
+      <c r="L5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="10" t="s">
+      <c r="N5" s="38"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="35"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="12" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="28" t="s">
+      <c r="O6" s="1"/>
+      <c r="P6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C7" s="13">
+      <c r="C7" s="9">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="M7" s="18">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="M7" s="14">
         <v>1</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="18">
         <v>1</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="29">
+      <c r="O7" s="1"/>
+      <c r="P7" s="24">
         <f>SUM(M7:O7)</f>
         <v>2</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="17">
         <f t="shared" ref="Q7:Q12" si="0">2-P7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C8" s="16">
+      <c r="C8" s="12">
         <f>C7+1</f>
         <v>2</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="M8" s="32">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="M8" s="27">
         <v>0</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="20">
         <v>1</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="30">
-        <f t="shared" ref="P8:P13" si="1">SUM(M8:O8)</f>
+      <c r="O8" s="1"/>
+      <c r="P8" s="25">
+        <f t="shared" ref="P8:P12" si="1">SUM(M8:O8)</f>
         <v>1</v>
       </c>
-      <c r="Q8" s="24">
+      <c r="Q8" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <f t="shared" ref="C9:C13" si="2">C8+1</f>
         <v>3</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="M9" s="18">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="M9" s="14">
         <v>0</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="18">
         <v>1</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="29">
+      <c r="O9" s="1"/>
+      <c r="P9" s="24">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C10" s="16">
+      <c r="C10" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="M10" s="32">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="M10" s="27">
         <v>1</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="20">
         <v>1</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="30">
+      <c r="O10" s="1"/>
+      <c r="P10" s="25">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q10" s="24">
+      <c r="Q10" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="M11" s="18">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="M11" s="14">
         <v>1</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="18">
         <v>1</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="29">
+      <c r="O11" s="1"/>
+      <c r="P11" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C12" s="16">
+      <c r="C12" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="M12" s="32">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="M12" s="27">
         <v>1</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="20">
         <v>0</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="30">
+      <c r="O12" s="1"/>
+      <c r="P12" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="24">
+      <c r="Q12" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="M13" s="18">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="14">
         <v>1</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="18">
         <v>1</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="29">
+      <c r="O13" s="1"/>
+      <c r="P13" s="24">
         <f>SUM(M13:O13)</f>
         <v>2</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="17">
         <f>2-P13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="N25" s="5"/>
+      <c r="N25" s="4"/>
     </row>
     <row r="32" spans="3:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="49" spans="3:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A65" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="7"/>
-      <c r="L65" s="11" t="s">
+      <c r="B65" s="36"/>
+      <c r="L65" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M65" s="33"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="2"/>
-      <c r="P65" s="10" t="s">
+      <c r="M65" s="28"/>
+      <c r="N65" s="29"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="Q65" s="10"/>
+      <c r="Q65" s="35"/>
+      <c r="R65" s="35"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="12" t="s">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A66" s="36"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="35"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="L66" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M66" s="31" t="s">
+      <c r="M66" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="N66" s="27" t="s">
+      <c r="N66" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O66" s="2"/>
-      <c r="P66" s="28" t="s">
+      <c r="O66" s="1"/>
+      <c r="P66" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Q66" s="26" t="s">
+      <c r="Q66" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="R66" s="39" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C67" s="13">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C67" s="9">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="29"/>
-      <c r="Q67" s="22"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="24"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C68" s="16">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C68" s="12">
         <f>C67+1</f>
         <v>2</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-      <c r="M68" s="32"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="30"/>
-      <c r="Q68" s="24"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="M68" s="27"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="25"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C69" s="13">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C69" s="9">
         <f t="shared" ref="C69:C76" si="3">C68+1</f>
         <v>3</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15"/>
-      <c r="M69" s="18"/>
-      <c r="N69" s="23"/>
-      <c r="O69" s="2"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="22"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="17"/>
+      <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C70" s="16">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C70" s="12">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
-      <c r="K70" s="18"/>
-      <c r="M70" s="32"/>
-      <c r="N70" s="25"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="30"/>
-      <c r="Q70" s="24"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="M70" s="27"/>
+      <c r="N70" s="20"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="25"/>
+      <c r="Q70" s="19"/>
+      <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C71" s="13">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C71" s="9">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="D71" s="20" t="s">
+      <c r="D71" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="15"/>
-      <c r="M71" s="18"/>
-      <c r="N71" s="23"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="29"/>
-      <c r="Q71" s="22"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="17"/>
+      <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C72" s="16">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C72" s="12">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-      <c r="M72" s="32"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="2"/>
-      <c r="P72" s="30"/>
-      <c r="Q72" s="24"/>
+      <c r="D72" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="25"/>
+      <c r="Q72" s="19"/>
+      <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C73" s="13">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C73" s="9">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="D73" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="15"/>
-      <c r="M73" s="18"/>
-      <c r="N73" s="23"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="29"/>
-      <c r="Q73" s="22"/>
+      <c r="D73" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="17"/>
+      <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C74" s="16">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C74" s="12">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="D74" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="25"/>
-      <c r="P74" s="37"/>
-      <c r="Q74" s="38"/>
+      <c r="D74" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="M74" s="27"/>
+      <c r="N74" s="20"/>
+      <c r="P74" s="32"/>
+      <c r="Q74" s="33"/>
+      <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C75" s="13">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C75" s="9">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="D75" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="M75" s="18"/>
-      <c r="N75" s="23"/>
-      <c r="P75" s="35"/>
-      <c r="Q75" s="36"/>
+      <c r="D75" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="11"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="18"/>
+      <c r="P75" s="30"/>
+      <c r="Q75" s="31"/>
+      <c r="R75" s="40"/>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C76" s="16">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C76" s="12">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="D76" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="M76" s="32"/>
-      <c r="N76" s="25"/>
-      <c r="P76" s="37"/>
-      <c r="Q76" s="38"/>
+      <c r="D76" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="M76" s="27"/>
+      <c r="N76" s="20"/>
+      <c r="P76" s="32"/>
+      <c r="Q76" s="33"/>
+      <c r="R76" s="41"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C77" s="13"/>
-      <c r="D77" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="M77" s="18"/>
-      <c r="N77" s="23"/>
-      <c r="P77" s="35"/>
-      <c r="Q77" s="36"/>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C77" s="9"/>
+      <c r="D77" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="18"/>
+      <c r="P77" s="30"/>
+      <c r="Q77" s="31"/>
+      <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C78" s="16">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C78" s="12">
         <v>11</v>
       </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="17" t="s">
+      <c r="D78" s="15"/>
+      <c r="E78" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-      <c r="M78" s="32"/>
-      <c r="N78" s="25"/>
-      <c r="P78" s="37"/>
-      <c r="Q78" s="38"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="M78" s="27"/>
+      <c r="N78" s="20"/>
+      <c r="P78" s="32"/>
+      <c r="Q78" s="33"/>
+      <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C79" s="13">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C79" s="9">
         <f>C78+1</f>
         <v>12</v>
       </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="14" t="s">
+      <c r="D79" s="16"/>
+      <c r="E79" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="M79" s="18"/>
-      <c r="N79" s="23"/>
-      <c r="P79" s="35"/>
-      <c r="Q79" s="36"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
+      <c r="M79" s="14"/>
+      <c r="N79" s="18"/>
+      <c r="P79" s="30"/>
+      <c r="Q79" s="31"/>
+      <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C80" s="16">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C80" s="12">
         <f>C79+1</f>
         <v>13</v>
       </c>
-      <c r="D80" s="19"/>
-      <c r="E80" s="17" t="s">
+      <c r="D80" s="15"/>
+      <c r="E80" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-      <c r="M80" s="32"/>
-      <c r="N80" s="25"/>
-      <c r="P80" s="37"/>
-      <c r="Q80" s="38"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="M80" s="27"/>
+      <c r="N80" s="20"/>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="33"/>
+      <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C81" s="13"/>
-      <c r="D81" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="20"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="M81" s="18"/>
-      <c r="N81" s="23"/>
-      <c r="P81" s="35"/>
-      <c r="Q81" s="36"/>
+    <row r="81" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C81" s="9"/>
+      <c r="D81" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E81" s="10"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="11"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="18"/>
+      <c r="P81" s="30"/>
+      <c r="Q81" s="31"/>
+      <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C82" s="16">
+    <row r="82" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C82" s="12">
         <v>14</v>
       </c>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19" t="s">
+      <c r="D82" s="15"/>
+      <c r="E82" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F82" s="18"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="18"/>
-      <c r="M82" s="32"/>
-      <c r="N82" s="25"/>
-      <c r="P82" s="37"/>
-      <c r="Q82" s="38"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="M82" s="27"/>
+      <c r="N82" s="20"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="33"/>
+      <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C83" s="13">
+    <row r="83" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C83" s="9">
         <f>C82+1</f>
         <v>15</v>
       </c>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20" t="s">
+      <c r="D83" s="16"/>
+      <c r="E83" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F83" s="15"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="M83" s="18"/>
-      <c r="N83" s="23"/>
-      <c r="P83" s="35"/>
-      <c r="Q83" s="36"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="18"/>
+      <c r="P83" s="30"/>
+      <c r="Q83" s="31"/>
+      <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C84" s="16">
+    <row r="84" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C84" s="12">
         <f>C83+1</f>
         <v>16</v>
       </c>
-      <c r="D84" s="18"/>
-      <c r="E84" s="19" t="s">
+      <c r="D84" s="14"/>
+      <c r="E84" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
-      <c r="J84" s="18"/>
-      <c r="K84" s="18"/>
-      <c r="M84" s="32"/>
-      <c r="N84" s="25"/>
-      <c r="P84" s="37"/>
-      <c r="Q84" s="38"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="M84" s="27"/>
+      <c r="N84" s="20"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="33"/>
+      <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="E85" s="3"/>
+    <row r="85" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C85" s="9">
+        <f>C84+1</f>
+        <v>17</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="16"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="M85" s="14"/>
+      <c r="N85" s="18"/>
+      <c r="P85" s="30"/>
+      <c r="Q85" s="31"/>
+      <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="E86" s="3"/>
+    <row r="86" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="E87" s="3"/>
+    <row r="87" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="E87" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="D66:K66"/>
-    <mergeCell ref="D6:K6"/>
     <mergeCell ref="F1:J3"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="P65:R65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update dos gráficos para prezi
</commit_message>
<xml_diff>
--- a/dados dos inquéritos.xlsx
+++ b/dados dos inquéritos.xlsx
@@ -564,20 +564,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1289,11 +1289,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1252558864"/>
-        <c:axId val="1252560912"/>
+        <c:axId val="1252555712"/>
+        <c:axId val="1252949520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1252558864"/>
+        <c:axId val="1252555712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,7 +1341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252560912"/>
+        <c:crossAx val="1252949520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1349,7 +1349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1252560912"/>
+        <c:axId val="1252949520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252558864"/>
+        <c:crossAx val="1252555712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1728,11 +1728,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1167222192"/>
-        <c:axId val="1167224512"/>
+        <c:axId val="1166086560"/>
+        <c:axId val="1251257552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1167222192"/>
+        <c:axId val="1166086560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167224512"/>
+        <c:crossAx val="1251257552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1788,7 +1788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1167224512"/>
+        <c:axId val="1251257552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167222192"/>
+        <c:crossAx val="1166086560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1972,6 +1972,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2095,6 +2096,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2210,6 +2212,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2333,6 +2336,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2448,6 +2452,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2571,6 +2576,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2686,6 +2692,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2809,6 +2816,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2924,6 +2932,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3047,6 +3056,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3162,6 +3172,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3285,6 +3296,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3400,6 +3412,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3523,6 +3536,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3878,6 +3892,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4001,6 +4016,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4116,6 +4132,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4287,11 +4304,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1251825168"/>
-        <c:axId val="1251950912"/>
+        <c:axId val="1252206496"/>
+        <c:axId val="1252558864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1251825168"/>
+        <c:axId val="1252206496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4339,7 +4356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1251950912"/>
+        <c:crossAx val="1252558864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4347,7 +4364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1251950912"/>
+        <c:axId val="1252558864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4403,7 +4420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1251825168"/>
+        <c:crossAx val="1252206496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4417,6 +4434,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4532,6 +4550,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4703,11 +4722,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1167303856"/>
-        <c:axId val="1167305632"/>
+        <c:axId val="1252078672"/>
+        <c:axId val="1252594368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1167303856"/>
+        <c:axId val="1252078672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4755,7 +4774,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167305632"/>
+        <c:crossAx val="1252594368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4763,7 +4782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1167305632"/>
+        <c:axId val="1252594368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4819,7 +4838,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167303856"/>
+        <c:crossAx val="1252078672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4833,6 +4852,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4948,6 +4968,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5071,6 +5092,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5906,6 +5928,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6029,6 +6052,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6144,6 +6168,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6267,6 +6292,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6382,6 +6408,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6505,6 +6532,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6620,6 +6648,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6743,6 +6772,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20566,8 +20596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="89" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="89" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20581,24 +20611,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
       <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
       <c r="M2" s="1">
         <v>1</v>
       </c>
@@ -20608,11 +20638,11 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
       <c r="M3" s="1">
         <v>0</v>
       </c>
@@ -20622,22 +20652,22 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M5" s="58" t="s">
+      <c r="M5" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="58"/>
-      <c r="O5" s="57" t="s">
+      <c r="N5" s="55"/>
+      <c r="O5" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="58" t="s">
+      <c r="P5" s="55" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1"/>
@@ -20650,15 +20680,15 @@
       <c r="L6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="58"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="55"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="54" t="s">
+      <c r="R6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="54"/>
+      <c r="S6" s="56"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
@@ -20666,16 +20696,16 @@
       <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="8" t="s">
         <v>1</v>
       </c>
@@ -20971,11 +21001,11 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="3:16" ht="19" x14ac:dyDescent="0.2">
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.2">
       <c r="N26" s="4"/>
@@ -20983,12 +21013,12 @@
       <c r="P26" s="4"/>
     </row>
     <row r="33" spans="3:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
     </row>
     <row r="49" spans="3:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C49" s="28" t="s">
@@ -21011,11 +21041,11 @@
       <c r="O66" s="34"/>
       <c r="P66" s="34"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="54" t="s">
+      <c r="R66" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="S66" s="54"/>
-      <c r="T66" s="54"/>
+      <c r="S66" s="56"/>
+      <c r="T66" s="56"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="53"/>
@@ -21023,16 +21053,16 @@
       <c r="C67" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="54" t="s">
+      <c r="D67" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="54"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
+      <c r="H67" s="56"/>
+      <c r="I67" s="56"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="56"/>
       <c r="L67" s="33">
         <v>5</v>
       </c>
@@ -21589,11 +21619,11 @@
       <c r="T87" s="1"/>
     </row>
     <row r="88" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C88" s="55" t="s">
+      <c r="C88" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
+      <c r="D88" s="58"/>
+      <c r="E88" s="58"/>
       <c r="G88" s="33"/>
       <c r="H88" s="33"/>
       <c r="I88" s="33"/>
@@ -21850,12 +21880,12 @@
       <c r="T103" s="1"/>
     </row>
     <row r="104" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C104" s="55" t="s">
+      <c r="C104" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D104" s="55"/>
-      <c r="E104" s="55"/>
-      <c r="F104" s="55"/>
+      <c r="D104" s="58"/>
+      <c r="E104" s="58"/>
+      <c r="F104" s="58"/>
       <c r="G104" s="33"/>
       <c r="H104" s="33"/>
       <c r="I104" s="33"/>
@@ -23044,10 +23074,10 @@
       <c r="O165" s="34"/>
       <c r="P165" s="34"/>
       <c r="Q165" s="1"/>
-      <c r="R165" s="54" t="s">
+      <c r="R165" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="S165" s="54"/>
+      <c r="S165" s="56"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="53"/>
@@ -23055,16 +23085,16 @@
       <c r="C166" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D166" s="54" t="s">
+      <c r="D166" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E166" s="54"/>
-      <c r="F166" s="54"/>
-      <c r="G166" s="54"/>
-      <c r="H166" s="54"/>
-      <c r="I166" s="54"/>
-      <c r="J166" s="54"/>
-      <c r="K166" s="54"/>
+      <c r="E166" s="56"/>
+      <c r="F166" s="56"/>
+      <c r="G166" s="56"/>
+      <c r="H166" s="56"/>
+      <c r="I166" s="56"/>
+      <c r="J166" s="56"/>
+      <c r="K166" s="56"/>
       <c r="L166" s="33">
         <v>2</v>
       </c>
@@ -23411,11 +23441,11 @@
       <c r="S180" s="1"/>
     </row>
     <row r="181" spans="3:19" ht="19" x14ac:dyDescent="0.2">
-      <c r="C181" s="55" t="s">
+      <c r="C181" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D181" s="55"/>
-      <c r="E181" s="55"/>
+      <c r="D181" s="58"/>
+      <c r="E181" s="58"/>
     </row>
     <row r="190" spans="3:19" x14ac:dyDescent="0.2">
       <c r="N190" s="4"/>
@@ -23423,12 +23453,12 @@
       <c r="P190" s="4"/>
     </row>
     <row r="197" spans="1:19" ht="19" x14ac:dyDescent="0.2">
-      <c r="C197" s="55" t="s">
+      <c r="C197" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D197" s="55"/>
-      <c r="E197" s="55"/>
-      <c r="F197" s="55"/>
+      <c r="D197" s="58"/>
+      <c r="E197" s="58"/>
+      <c r="F197" s="58"/>
     </row>
     <row r="198" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="47"/>
@@ -24034,11 +24064,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="A165:B166"/>
+    <mergeCell ref="R165:S165"/>
+    <mergeCell ref="D166:K166"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="D67:K67"/>
     <mergeCell ref="F1:J4"/>
     <mergeCell ref="C197:F197"/>
     <mergeCell ref="C104:F104"/>
@@ -24047,12 +24078,11 @@
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C33:F33"/>
-    <mergeCell ref="A165:B166"/>
-    <mergeCell ref="R165:S165"/>
-    <mergeCell ref="D166:K166"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="A66:B67"/>
-    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
+ 1 associação e + 16 voluntarios/canis
</commit_message>
<xml_diff>
--- a/dados dos inquéritos.xlsx
+++ b/dados dos inquéritos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Inquéritos p/ o Projeto de Inovação</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Clínica Veterinária Animal Especial</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -564,20 +567,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -880,6 +883,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -976,7 +980,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1003,6 +1007,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1118,6 +1123,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1207,7 +1213,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -1270,10 +1276,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,11 +1295,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1252555712"/>
-        <c:axId val="1252949520"/>
+        <c:axId val="501961520"/>
+        <c:axId val="502737872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1252555712"/>
+        <c:axId val="501961520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,7 +1347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252949520"/>
+        <c:crossAx val="502737872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1349,7 +1355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1252949520"/>
+        <c:axId val="502737872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252555712"/>
+        <c:crossAx val="501961520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1418,6 +1424,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1533,6 +1540,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1628,10 +1636,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -1706,13 +1714,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1728,11 +1736,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1166086560"/>
-        <c:axId val="1251257552"/>
+        <c:axId val="588301248"/>
+        <c:axId val="588304000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1166086560"/>
+        <c:axId val="588301248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1251257552"/>
+        <c:crossAx val="588304000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1788,7 +1796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1251257552"/>
+        <c:axId val="588304000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1851,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1166086560"/>
+        <c:crossAx val="588301248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1857,6 +1865,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2066,7 +2075,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -2306,10 +2315,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2546,10 +2555,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2786,10 +2795,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3026,10 +3035,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3266,10 +3275,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3506,10 +3515,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3986,10 +3995,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4222,13 +4231,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4282,13 +4291,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4304,11 +4313,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1252206496"/>
-        <c:axId val="1252558864"/>
+        <c:axId val="588441568"/>
+        <c:axId val="588444320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1252206496"/>
+        <c:axId val="588441568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252558864"/>
+        <c:crossAx val="588444320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4364,7 +4373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1252558864"/>
+        <c:axId val="588444320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4420,7 +4429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252206496"/>
+        <c:crossAx val="588441568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4640,13 +4649,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4700,13 +4709,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4722,11 +4731,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1252078672"/>
-        <c:axId val="1252594368"/>
+        <c:axId val="588474112"/>
+        <c:axId val="588476864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1252078672"/>
+        <c:axId val="588474112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4774,7 +4783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252594368"/>
+        <c:crossAx val="588476864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4782,7 +4791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1252594368"/>
+        <c:axId val="588476864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4838,7 +4847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1252078672"/>
+        <c:crossAx val="588474112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5065,7 +5074,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6502,7 +6511,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -6742,7 +6751,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -20596,8 +20605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="89" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M175" sqref="M175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20611,24 +20620,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
       <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
       <c r="M2" s="1">
         <v>1</v>
       </c>
@@ -20638,11 +20647,11 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
       <c r="M3" s="1">
         <v>0</v>
       </c>
@@ -20652,22 +20661,22 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="54" t="s">
+      <c r="N5" s="58"/>
+      <c r="O5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="P5" s="58" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1"/>
@@ -20680,15 +20689,15 @@
       <c r="L6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="55"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="58"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="56" t="s">
+      <c r="R6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="56"/>
+      <c r="S6" s="54"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
@@ -20696,16 +20705,16 @@
       <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
       <c r="L7" s="8" t="s">
         <v>1</v>
       </c>
@@ -21001,11 +21010,11 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="3:16" ht="19" x14ac:dyDescent="0.2">
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.2">
       <c r="N26" s="4"/>
@@ -21013,12 +21022,12 @@
       <c r="P26" s="4"/>
     </row>
     <row r="33" spans="3:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
     </row>
     <row r="49" spans="3:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C49" s="28" t="s">
@@ -21041,11 +21050,11 @@
       <c r="O66" s="34"/>
       <c r="P66" s="34"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="56" t="s">
+      <c r="R66" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="S66" s="56"/>
-      <c r="T66" s="56"/>
+      <c r="S66" s="54"/>
+      <c r="T66" s="54"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="53"/>
@@ -21053,18 +21062,18 @@
       <c r="C67" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="56" t="s">
+      <c r="D67" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="56"/>
-      <c r="I67" s="56"/>
-      <c r="J67" s="56"/>
-      <c r="K67" s="56"/>
+      <c r="E67" s="54"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
+      <c r="I67" s="54"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="54"/>
       <c r="L67" s="33">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="M67" s="33"/>
       <c r="N67" s="33"/>
@@ -21102,7 +21111,7 @@
       <c r="P68" s="33"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="29">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="S68" s="17">
         <f>$L$67-R68</f>
@@ -21131,11 +21140,11 @@
       <c r="P69" s="33"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="25">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="S69" s="19">
         <f t="shared" ref="S69:S86" si="3">$L$67-R69</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T69" s="1"/>
     </row>
@@ -21160,11 +21169,11 @@
       <c r="P70" s="33"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S70" s="17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="T70" s="1"/>
     </row>
@@ -21189,11 +21198,11 @@
       <c r="P71" s="33"/>
       <c r="Q71" s="1"/>
       <c r="R71" s="25">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S71" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T71" s="1"/>
     </row>
@@ -21218,11 +21227,11 @@
       <c r="P72" s="33"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="29">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S72" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T72" s="1"/>
     </row>
@@ -21247,11 +21256,11 @@
       <c r="P73" s="33"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S73" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="T73" s="1"/>
     </row>
@@ -21276,11 +21285,11 @@
       <c r="P74" s="33"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S74" s="17">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="T74" s="1"/>
     </row>
@@ -21304,11 +21313,11 @@
       <c r="O75" s="33"/>
       <c r="P75" s="33"/>
       <c r="R75" s="52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S75" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="T75" s="1"/>
     </row>
@@ -21402,11 +21411,11 @@
       <c r="O79" s="33"/>
       <c r="P79" s="33"/>
       <c r="R79" s="52">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S79" s="19">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="T79" s="1"/>
     </row>
@@ -21430,11 +21439,11 @@
       <c r="O80" s="33"/>
       <c r="P80" s="33"/>
       <c r="R80" s="50">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="S80" s="17">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T80" s="1"/>
     </row>
@@ -21458,11 +21467,11 @@
       <c r="O81" s="33"/>
       <c r="P81" s="33"/>
       <c r="R81" s="52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S81" s="19">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="T81" s="1"/>
     </row>
@@ -21506,11 +21515,11 @@
       <c r="O83" s="33"/>
       <c r="P83" s="33"/>
       <c r="R83" s="52">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="S83" s="19">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="T83" s="1"/>
     </row>
@@ -21534,11 +21543,11 @@
       <c r="O84" s="33"/>
       <c r="P84" s="33"/>
       <c r="R84" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S84" s="17">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="T84" s="1"/>
     </row>
@@ -21562,11 +21571,11 @@
       <c r="O85" s="33"/>
       <c r="P85" s="33"/>
       <c r="R85" s="52">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="S85" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="T85" s="1"/>
     </row>
@@ -21594,7 +21603,7 @@
       </c>
       <c r="S86" s="17">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="T86" s="1"/>
     </row>
@@ -21619,11 +21628,11 @@
       <c r="T87" s="1"/>
     </row>
     <row r="88" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C88" s="58" t="s">
+      <c r="C88" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="58"/>
-      <c r="E88" s="58"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
       <c r="G88" s="33"/>
       <c r="H88" s="33"/>
       <c r="I88" s="33"/>
@@ -21880,12 +21889,12 @@
       <c r="T103" s="1"/>
     </row>
     <row r="104" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C104" s="58" t="s">
+      <c r="C104" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D104" s="58"/>
-      <c r="E104" s="58"/>
-      <c r="F104" s="58"/>
+      <c r="D104" s="55"/>
+      <c r="E104" s="55"/>
+      <c r="F104" s="55"/>
       <c r="G104" s="33"/>
       <c r="H104" s="33"/>
       <c r="I104" s="33"/>
@@ -23074,10 +23083,10 @@
       <c r="O165" s="34"/>
       <c r="P165" s="34"/>
       <c r="Q165" s="1"/>
-      <c r="R165" s="56" t="s">
+      <c r="R165" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="S165" s="56"/>
+      <c r="S165" s="54"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="53"/>
@@ -23085,18 +23094,18 @@
       <c r="C166" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D166" s="56" t="s">
+      <c r="D166" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E166" s="56"/>
-      <c r="F166" s="56"/>
-      <c r="G166" s="56"/>
-      <c r="H166" s="56"/>
-      <c r="I166" s="56"/>
-      <c r="J166" s="56"/>
-      <c r="K166" s="56"/>
+      <c r="E166" s="54"/>
+      <c r="F166" s="54"/>
+      <c r="G166" s="54"/>
+      <c r="H166" s="54"/>
+      <c r="I166" s="54"/>
+      <c r="J166" s="54"/>
+      <c r="K166" s="54"/>
       <c r="L166" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M166" s="34"/>
       <c r="N166" s="33"/>
@@ -23133,7 +23142,7 @@
       <c r="P167" s="33"/>
       <c r="Q167" s="1"/>
       <c r="R167" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S167" s="37">
         <f>$L$166-R167</f>
@@ -23163,7 +23172,7 @@
       <c r="P168" s="33"/>
       <c r="Q168" s="1"/>
       <c r="R168" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S168" s="38">
         <f>$L$166-R168</f>
@@ -23185,7 +23194,9 @@
       <c r="I169" s="11"/>
       <c r="J169" s="11"/>
       <c r="K169" s="11"/>
-      <c r="M169" s="33"/>
+      <c r="M169" s="33" t="s">
+        <v>62</v>
+      </c>
       <c r="N169" s="33"/>
       <c r="O169" s="33"/>
       <c r="P169" s="33"/>
@@ -23195,7 +23206,7 @@
       </c>
       <c r="S169" s="37">
         <f>$L$166-R169</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.2">
@@ -23237,7 +23248,7 @@
       <c r="O171" s="33"/>
       <c r="P171" s="33"/>
       <c r="R171" s="40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S171" s="37">
         <f>$L$166-R171</f>
@@ -23269,7 +23280,7 @@
       </c>
       <c r="S172" s="38">
         <f>$L$166-R172</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T172" s="1"/>
     </row>
@@ -23297,7 +23308,7 @@
       </c>
       <c r="S173" s="37">
         <f>$L$166-R173</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T173" s="1"/>
     </row>
@@ -23333,7 +23344,7 @@
       <c r="K175" s="11"/>
       <c r="Q175" s="1"/>
       <c r="R175" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S175" s="37">
         <f>$L$166-R175</f>
@@ -23357,7 +23368,7 @@
       <c r="K176" s="14"/>
       <c r="Q176" s="1"/>
       <c r="R176" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S176" s="38">
         <f>$L$166-R176</f>
@@ -23385,7 +23396,7 @@
       </c>
       <c r="S177" s="37">
         <f>$L$166-R177</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="3:19" x14ac:dyDescent="0.2">
@@ -23409,7 +23420,7 @@
       </c>
       <c r="S178" s="38">
         <f>$L$166-R178</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="3:19" x14ac:dyDescent="0.2">
@@ -23433,7 +23444,7 @@
       </c>
       <c r="S179" s="37">
         <f>$L$166-R179</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="3:19" x14ac:dyDescent="0.2">
@@ -23441,11 +23452,11 @@
       <c r="S180" s="1"/>
     </row>
     <row r="181" spans="3:19" ht="19" x14ac:dyDescent="0.2">
-      <c r="C181" s="58" t="s">
+      <c r="C181" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D181" s="58"/>
-      <c r="E181" s="58"/>
+      <c r="D181" s="55"/>
+      <c r="E181" s="55"/>
     </row>
     <row r="190" spans="3:19" x14ac:dyDescent="0.2">
       <c r="N190" s="4"/>
@@ -23453,12 +23464,12 @@
       <c r="P190" s="4"/>
     </row>
     <row r="197" spans="1:19" ht="19" x14ac:dyDescent="0.2">
-      <c r="C197" s="58" t="s">
+      <c r="C197" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D197" s="58"/>
-      <c r="E197" s="58"/>
-      <c r="F197" s="58"/>
+      <c r="D197" s="55"/>
+      <c r="E197" s="55"/>
+      <c r="F197" s="55"/>
     </row>
     <row r="198" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="47"/>
@@ -24064,12 +24075,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A165:B166"/>
-    <mergeCell ref="R165:S165"/>
-    <mergeCell ref="D166:K166"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="A66:B67"/>
-    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="F1:J4"/>
     <mergeCell ref="C197:F197"/>
     <mergeCell ref="C104:F104"/>
@@ -24078,11 +24088,12 @@
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C33:F33"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="A165:B166"/>
+    <mergeCell ref="R165:S165"/>
+    <mergeCell ref="D166:K166"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="D67:K67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Inqueritos Parceiros e 1 parceiro
</commit_message>
<xml_diff>
--- a/dados dos inquéritos.xlsx
+++ b/dados dos inquéritos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Inquéritos p/ o Projeto de Inovação</t>
   </si>
@@ -263,14 +263,36 @@
   <si>
     <t>Enf Fernanda Portillo</t>
   </si>
+  <si>
+    <t>Parceiros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quanto estaria disposto a pagar mensalmente?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estaria disposto a contribuir com campanhas de desconto para os animais adotados através da plataforma? </t>
+  </si>
+  <si>
+    <t>Total Parceiros</t>
+  </si>
+  <si>
+    <t>Mania dos Cães</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -323,8 +345,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +468,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -449,12 +489,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -537,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -589,16 +631,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -613,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -625,14 +667,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="40% - Cor1" xfId="3" builtinId="31"/>
+    <cellStyle name="Cor5" xfId="4" builtinId="45"/>
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,6 +1103,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1304,6 +1355,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1404,6 +1456,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1680,6 +1733,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4358,6 +4412,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4443,6 +4498,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4543,6 +4599,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4628,6 +4685,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4728,6 +4786,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4813,6 +4872,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -21708,10 +21768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X282"/>
+  <dimension ref="A1:X306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="89" workbookViewId="0">
+      <selection activeCell="R305" sqref="R305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -21720,7 +21780,7 @@
     <col min="3" max="3" width="10.875" style="5"/>
     <col min="4" max="10" width="10.875" style="1"/>
     <col min="11" max="11" width="23.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" style="1"/>
+    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
     <col min="13" max="16" width="17.625" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.625" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
@@ -25838,8 +25898,126 @@
       <c r="D282" s="59"/>
       <c r="E282" s="59"/>
     </row>
+    <row r="298" spans="1:16">
+      <c r="L298" s="42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16">
+      <c r="A299" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B299" s="54"/>
+      <c r="C299" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D299" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E299" s="57"/>
+      <c r="F299" s="57"/>
+      <c r="G299" s="57"/>
+      <c r="H299" s="57"/>
+      <c r="I299" s="57"/>
+      <c r="J299" s="57"/>
+      <c r="K299" s="57"/>
+      <c r="L299" s="1">
+        <v>1</v>
+      </c>
+      <c r="M299" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="P299" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16">
+      <c r="A300" s="54"/>
+      <c r="B300" s="54"/>
+      <c r="C300" s="9">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="D300" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E300" s="11"/>
+      <c r="F300" s="11"/>
+      <c r="G300" s="11"/>
+      <c r="H300" s="11"/>
+      <c r="I300" s="11"/>
+      <c r="J300" s="11"/>
+      <c r="K300" s="11"/>
+      <c r="M300" s="14">
+        <v>1</v>
+      </c>
+      <c r="P300" s="29">
+        <f>SUM(M300)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16">
+      <c r="C301" s="12">
+        <f>C300+1</f>
+        <v>2</v>
+      </c>
+      <c r="D301" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E301" s="14"/>
+      <c r="F301" s="14"/>
+      <c r="G301" s="14"/>
+      <c r="H301" s="14"/>
+      <c r="I301" s="14"/>
+      <c r="J301" s="14"/>
+      <c r="K301" s="14"/>
+      <c r="M301" s="27">
+        <v>1</v>
+      </c>
+      <c r="P301" s="61">
+        <f>SUM(M301)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16">
+      <c r="C302" s="9">
+        <f t="shared" ref="C302" si="10">C301+1</f>
+        <v>3</v>
+      </c>
+      <c r="D302" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E302" s="11"/>
+      <c r="F302" s="11"/>
+      <c r="G302" s="11"/>
+      <c r="H302" s="11"/>
+      <c r="I302" s="11"/>
+      <c r="J302" s="11"/>
+      <c r="K302" s="11"/>
+      <c r="M302" s="14">
+        <v>0</v>
+      </c>
+      <c r="P302" s="29">
+        <f>SUM(M302)/L299</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16">
+      <c r="P303"/>
+    </row>
+    <row r="304" spans="1:16">
+      <c r="P304"/>
+    </row>
+    <row r="305" spans="16:16">
+      <c r="P305"/>
+    </row>
+    <row r="306" spans="16:16">
+      <c r="P306"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
+    <mergeCell ref="D299:K299"/>
+    <mergeCell ref="A299:B300"/>
     <mergeCell ref="C282:E282"/>
     <mergeCell ref="A245:B246"/>
     <mergeCell ref="D246:K246"/>
@@ -25866,8 +26044,8 @@
     <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-  <picture r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <picture r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>